<commit_message>
presentation and report documents
</commit_message>
<xml_diff>
--- a/model_results/abalone_combined.xlsx
+++ b/model_results/abalone_combined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zackhorton/Documents/MIT/15.095_Machine_Learning/Project/ML-Project/model_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07D4752-9413-4441-8B7B-CA1A73198771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A3FB32-3122-354C-81C8-6546D4A6DE65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{5D31CEA5-B9F5-634B-A19C-B2CC2199DD56}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$649</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$649</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -179,7 +179,16 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8CBAD"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -492,7 +501,7 @@
   <dimension ref="A1:K649"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>